<commit_message>
modified formatting of team distribution
</commit_message>
<xml_diff>
--- a/SPRING 20/CSE 101 Non CSE/Section 4/team_dist_cse101_sec4.xlsx
+++ b/SPRING 20/CSE 101 Non CSE/Section 4/team_dist_cse101_sec4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\SPRING 20\CSE 101 Non CSE\Section 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEF7881-D3CF-4DDD-86DA-25FD1FCF334B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB8C8D2-9320-483B-8093-0F9D5B8D416C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -282,7 +282,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -314,15 +314,37 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -801,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView showOutlineSymbols="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView showOutlineSymbols="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1722,7 +1744,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:XFD47">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$E2 &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1737,595 +1759,595 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="30.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="14"/>
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="9" t="e">
+      <c r="B2" s="10" t="e">
         <f>VLOOKUP(A2,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D2" s="9" t="e">
+      <c r="D2" s="10" t="e">
         <f>B2</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="9" t="e">
+      <c r="B3" s="10" t="e">
         <f>VLOOKUP(A3,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D3" s="9" t="e">
+      <c r="D3" s="10" t="e">
         <f t="shared" ref="D3:D55" si="0">B3</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="9" t="e">
+      <c r="B4" s="10" t="e">
         <f>VLOOKUP(A4,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D4" s="9" t="e">
+      <c r="D4" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="e">
+      <c r="B5" s="10" t="e">
         <f>VLOOKUP(A5,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D5" s="9" t="e">
+      <c r="D5" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="e">
+      <c r="B6" s="10" t="e">
         <f>VLOOKUP(A6,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D6" s="9" t="e">
+      <c r="D6" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="e">
+      <c r="B8" s="10" t="e">
         <f>VLOOKUP(A8,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D8" s="9" t="e">
+      <c r="D8" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="e">
+      <c r="B9" s="10" t="e">
         <f>VLOOKUP(A9,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D9" s="9" t="e">
+      <c r="D9" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="e">
+      <c r="B10" s="10" t="e">
         <f>VLOOKUP(A10,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D10" s="9" t="e">
+      <c r="D10" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="e">
+      <c r="B11" s="10" t="e">
         <f>VLOOKUP(A11,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D11" s="9" t="e">
+      <c r="D11" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="e">
+      <c r="B12" s="10" t="e">
         <f>VLOOKUP(A12,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D12" s="9" t="e">
+      <c r="D12" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="9" t="e">
+      <c r="B14" s="10" t="e">
         <f>VLOOKUP(A14,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D14" s="9" t="e">
+      <c r="D14" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="e">
+      <c r="B15" s="10" t="e">
         <f>VLOOKUP(A15,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D15" s="9" t="e">
+      <c r="D15" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="e">
+      <c r="B16" s="10" t="e">
         <f>VLOOKUP(A16,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D16" s="9" t="e">
+      <c r="D16" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="e">
+      <c r="B17" s="10" t="e">
         <f>VLOOKUP(A17,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D17" s="9" t="e">
+      <c r="D17" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="e">
+      <c r="B18" s="10" t="e">
         <f>VLOOKUP(A18,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D18" s="9" t="e">
+      <c r="D18" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="e">
+      <c r="B20" s="10" t="e">
         <f>VLOOKUP(A20,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D20" s="9" t="e">
+      <c r="D20" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="e">
+      <c r="B21" s="10" t="e">
         <f>VLOOKUP(A21,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D21" s="9" t="e">
+      <c r="D21" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="9" t="e">
+      <c r="B22" s="10" t="e">
         <f>VLOOKUP(A22,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D22" s="9" t="e">
+      <c r="D22" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="e">
+      <c r="B23" s="10" t="e">
         <f>VLOOKUP(A23,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D23" s="9" t="e">
+      <c r="D23" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="e">
+      <c r="B24" s="10" t="e">
         <f>VLOOKUP(A24,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D24" s="9" t="e">
+      <c r="D24" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="9" t="e">
+      <c r="B26" s="10" t="e">
         <f>VLOOKUP(A26,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D26" s="9" t="e">
+      <c r="D26" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="e">
+      <c r="B27" s="10" t="e">
         <f>VLOOKUP(A27,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D27" s="9" t="e">
+      <c r="D27" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="9" t="e">
+      <c r="B28" s="10" t="e">
         <f>VLOOKUP(A28,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D28" s="9" t="e">
+      <c r="D28" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="9" t="e">
+      <c r="B29" s="10" t="e">
         <f>VLOOKUP(A29,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D29" s="9" t="e">
+      <c r="D29" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="e">
+      <c r="B30" s="10" t="e">
         <f>VLOOKUP(A30,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D30" s="9" t="e">
+      <c r="D30" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="15"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="9" t="e">
+      <c r="B32" s="10" t="e">
         <f>VLOOKUP(A32,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D32" s="9" t="e">
+      <c r="D32" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="9" t="e">
+      <c r="B33" s="10" t="e">
         <f>VLOOKUP(A33,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D33" s="9" t="e">
+      <c r="D33" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="9" t="e">
+      <c r="B34" s="10" t="e">
         <f>VLOOKUP(A34,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D34" s="9" t="e">
+      <c r="D34" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="e">
+      <c r="B35" s="10" t="e">
         <f>VLOOKUP(A35,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D35" s="9" t="e">
+      <c r="D35" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="9" t="e">
+      <c r="B36" s="10" t="e">
         <f>VLOOKUP(A36,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D36" s="9" t="e">
+      <c r="D36" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="15"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="9" t="e">
+      <c r="B38" s="10" t="e">
         <f>VLOOKUP(A38,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D38" s="9" t="e">
+      <c r="D38" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="e">
+      <c r="B39" s="10" t="e">
         <f>VLOOKUP(A39,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D39" s="9" t="e">
+      <c r="D39" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="9" t="e">
+      <c r="B40" s="10" t="e">
         <f>VLOOKUP(A40,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D40" s="9" t="e">
+      <c r="D40" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="9" t="e">
+      <c r="B41" s="10" t="e">
         <f>VLOOKUP(A41,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D41" s="9" t="e">
+      <c r="D41" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="9" t="e">
+      <c r="B42" s="10" t="e">
         <f>VLOOKUP(A42,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D42" s="9" t="e">
+      <c r="D42" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="15"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="9" t="e">
+      <c r="B44" s="10" t="e">
         <f>VLOOKUP(A44,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D44" s="9" t="e">
+      <c r="D44" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="9" t="e">
+      <c r="B45" s="10" t="e">
         <f>VLOOKUP(A45,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D45" s="9" t="e">
+      <c r="D45" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="9" t="e">
+      <c r="B46" s="10" t="e">
         <f>VLOOKUP(A46,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D46" s="9" t="e">
+      <c r="D46" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="9" t="e">
+      <c r="B47" s="10" t="e">
         <f>VLOOKUP(A47,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D47" s="9" t="e">
+      <c r="D47" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="9" t="e">
+      <c r="B48" s="10" t="e">
         <f>VLOOKUP(A48,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D48" s="9" t="e">
+      <c r="D48" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="15"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="9" t="e">
+      <c r="B50" s="10" t="e">
         <f>VLOOKUP(A50,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D50" s="9" t="e">
+      <c r="D50" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="9" t="e">
+      <c r="B51" s="10" t="e">
         <f>VLOOKUP(A51,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D51" s="9" t="e">
+      <c r="D51" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="9" t="e">
+      <c r="B52" s="10" t="e">
         <f>VLOOKUP(A52,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D52" s="9" t="e">
+      <c r="D52" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="9" t="e">
+      <c r="B53" s="10" t="e">
         <f>VLOOKUP(A53,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D53" s="9" t="e">
+      <c r="D53" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="9" t="e">
+      <c r="B54" s="10" t="e">
         <f>VLOOKUP(A54,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D54" s="9" t="e">
+      <c r="D54" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="9" t="e">
+      <c r="B55" s="10" t="e">
         <f>VLOOKUP(A55,name_id!C$2:D$47,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D55" s="9" t="e">
+      <c r="D55" s="10" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
+      <c r="A56" s="12"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$E14</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>$E14&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" priority="9">
+    <cfRule type="expression" priority="10">
       <formula>$E14 &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$E33</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>$E33&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" priority="6">
+    <cfRule type="expression" priority="7">
       <formula>$E33 &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
+  <conditionalFormatting sqref="A22">
     <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$E55 &gt; 0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$E22 &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$E53 &gt; 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$E53 &gt; 0</formula>
+      <formula>$E55 &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>